<commit_message>
• Added results of database complexity metrics.
</commit_message>
<xml_diff>
--- a/Koli_2017/db_metrics.xlsx
+++ b/Koli_2017/db_metrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="50340" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="24">
   <si>
     <t>Entities</t>
   </si>
@@ -62,10 +62,43 @@
     <t>DCI</t>
   </si>
   <si>
-    <t>NFK</t>
-  </si>
-  <si>
     <t>DC</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>DRT</t>
+  </si>
+  <si>
+    <t>SMARtS</t>
+  </si>
+  <si>
+    <t>Simple data type field</t>
+  </si>
+  <si>
+    <t>Complex data type</t>
+  </si>
+  <si>
+    <t>Each field in primary key</t>
+  </si>
+  <si>
+    <t>Each field in foreign key</t>
+  </si>
+  <si>
+    <t>Assertion</t>
+  </si>
+  <si>
+    <t>One-to-one</t>
+  </si>
+  <si>
+    <t>One-to-many</t>
+  </si>
+  <si>
+    <t>Many-to-many</t>
   </si>
 </sst>
 </file>
@@ -121,8 +154,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -140,19 +213,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,34 +541,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J3:J8"/>
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -469,8 +601,21 @@
         <f>B4*C4</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4">
+        <v>32</v>
+      </c>
+      <c r="O4">
+        <v>0.25</v>
+      </c>
+      <c r="P4">
+        <f>O4*N4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -484,8 +629,21 @@
         <f t="shared" ref="D5:D8" si="0">B5*C5</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0.5</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P11" si="1">O5*N5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -499,8 +657,21 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6">
+        <v>9</v>
+      </c>
+      <c r="O6">
+        <v>0.25</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -514,8 +685,21 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7">
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>0.5</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -529,8 +713,21 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8">
+        <v>14</v>
+      </c>
+      <c r="O8">
+        <v>0.75</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D9">
         <f>SUM(D4:D8)</f>
         <v>277</v>
@@ -538,19 +735,72 @@
       <c r="F9">
         <v>9</v>
       </c>
+      <c r="G9">
+        <v>32</v>
+      </c>
       <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="J9">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>0.25</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10">
+        <v>3</v>
+      </c>
+      <c r="O10">
+        <v>0.5</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>0.75</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P12">
+        <f>SUM(P4:P11)</f>
+        <v>28.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -565,7 +815,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -576,11 +826,11 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D17" si="1">B14*C14</f>
+        <f t="shared" ref="D14:D17" si="2">B14*C14</f>
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -591,11 +841,17 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -606,11 +862,24 @@
         <v>5</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16">
+        <v>43</v>
+      </c>
+      <c r="O16">
+        <v>0.25</v>
+      </c>
+      <c r="P16">
+        <f>O16*N16</f>
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -621,11 +890,24 @@
         <v>3</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0.5</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17:P23" si="3">O17*N17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D18">
         <f>SUM(D13:D17)</f>
         <v>367</v>
@@ -633,19 +915,81 @@
       <c r="F18">
         <v>12</v>
       </c>
+      <c r="G18">
+        <v>43</v>
+      </c>
       <c r="H18">
+        <v>9</v>
+      </c>
+      <c r="J18">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18">
+        <v>12</v>
+      </c>
+      <c r="O18">
+        <v>0.25</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19">
+        <v>12</v>
+      </c>
+      <c r="O19">
+        <v>0.5</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20">
+        <v>18</v>
+      </c>
+      <c r="O20">
+        <v>0.75</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <v>0.25</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -659,8 +1003,21 @@
         <f>B22*C22</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22">
+        <v>9</v>
+      </c>
+      <c r="O22">
+        <v>0.5</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="3"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -674,8 +1031,21 @@
         <f>B23*C23</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M23" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0.75</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -689,8 +1059,12 @@
         <f>B24*C24</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P24">
+        <f>SUM(P16:P23)</f>
+        <v>38.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -705,7 +1079,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -720,7 +1094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D27">
         <f>SUM(D22:D26)</f>
         <v>370</v>
@@ -728,11 +1102,53 @@
       <c r="F27">
         <v>11</v>
       </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
       <c r="H27">
+        <v>8</v>
+      </c>
+      <c r="J27">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>8</v>
+      </c>
+      <c r="O27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M28" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28">
+        <v>48</v>
+      </c>
+      <c r="O28">
+        <v>0.25</v>
+      </c>
+      <c r="P28">
+        <f>O28*N28</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N29">
+        <v>2</v>
+      </c>
+      <c r="O29">
+        <v>0.5</v>
+      </c>
+      <c r="P29">
+        <f t="shared" ref="P29:P35" si="4">O29*N29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -741,8 +1157,21 @@
         <v>5</v>
       </c>
       <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M30" t="s">
+        <v>18</v>
+      </c>
+      <c r="N30">
+        <v>13</v>
+      </c>
+      <c r="O30">
+        <v>0.25</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="4"/>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,11 +1182,24 @@
         <v>15</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D35" si="2">B31*C31</f>
+        <f t="shared" ref="D31:D35" si="5">B31*C31</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M31" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31">
+        <v>11</v>
+      </c>
+      <c r="O31">
+        <v>0.5</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -768,11 +1210,24 @@
         <v>5</v>
       </c>
       <c r="D32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M32" t="s">
+        <v>20</v>
+      </c>
+      <c r="N32">
+        <v>18</v>
+      </c>
+      <c r="O32">
+        <v>0.75</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="4"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -783,11 +1238,24 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M33" t="s">
+        <v>21</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0.25</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -798,11 +1266,24 @@
         <v>5</v>
       </c>
       <c r="D34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M34" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34">
+        <v>11</v>
+      </c>
+      <c r="O34">
+        <v>0.5</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -813,11 +1294,24 @@
         <v>3</v>
       </c>
       <c r="D35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M35" t="s">
+        <v>23</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0.75</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -828,8 +1322,152 @@
       <c r="F36">
         <v>13</v>
       </c>
+      <c r="G36">
+        <v>46</v>
+      </c>
       <c r="H36">
+        <v>7</v>
+      </c>
+      <c r="J36">
         <v>53</v>
+      </c>
+      <c r="P36">
+        <f>SUM(P28:P35)</f>
+        <v>40.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M40" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40">
+        <v>46</v>
+      </c>
+      <c r="O40">
+        <v>0.25</v>
+      </c>
+      <c r="P40">
+        <f>O40*N40</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M41" t="s">
+        <v>17</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0.5</v>
+      </c>
+      <c r="P41">
+        <f t="shared" ref="P41:P47" si="6">O41*N41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M42" t="s">
+        <v>18</v>
+      </c>
+      <c r="N42">
+        <v>12</v>
+      </c>
+      <c r="O42">
+        <v>0.25</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M43" t="s">
+        <v>19</v>
+      </c>
+      <c r="N43">
+        <v>13</v>
+      </c>
+      <c r="O43">
+        <v>0.5</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="6"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N44">
+        <v>14</v>
+      </c>
+      <c r="O44">
+        <v>0.75</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="6"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M45" t="s">
+        <v>21</v>
+      </c>
+      <c r="N45">
+        <v>4</v>
+      </c>
+      <c r="O45">
+        <v>0.25</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M46" t="s">
+        <v>22</v>
+      </c>
+      <c r="N46">
+        <v>8</v>
+      </c>
+      <c r="O46">
+        <v>0.5</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M47" t="s">
+        <v>23</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0.75</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P48">
+        <f>SUM(P40:P47)</f>
+        <v>36.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>